<commit_message>
project is updated till add new customer
</commit_message>
<xml_diff>
--- a/src/test/java/com/inetbanking/TestData/LoginDataXL.xlsx
+++ b/src/test/java/com/inetbanking/TestData/LoginDataXL.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\inetBankingV1\src\test\java\com\inetbanking\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2440" windowWidth="15530" windowHeight="6140"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14260" windowHeight="3480"/>
   </bookViews>
   <sheets>
     <sheet name="LoginDetails" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Username</t>
   </si>
@@ -44,31 +49,13 @@
   </si>
   <si>
     <t>wertyuvb</t>
-  </si>
-  <si>
-    <t>TestCaseID</t>
-  </si>
-  <si>
-    <t>TC_001</t>
-  </si>
-  <si>
-    <t>TC_002</t>
-  </si>
-  <si>
-    <t>TC_003</t>
-  </si>
-  <si>
-    <t>TC_004</t>
-  </si>
-  <si>
-    <t>TC_005</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,6 +123,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -182,7 +177,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -214,9 +209,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -248,6 +244,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -423,83 +420,65 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>